<commit_message>
- adding witch base
</commit_message>
<xml_diff>
--- a/Character Stats.xlsx
+++ b/Character Stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Character" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="65">
   <si>
     <t>Class</t>
   </si>
@@ -166,6 +166,57 @@
   </si>
   <si>
     <t>4,8</t>
+  </si>
+  <si>
+    <t>Light Magic Skill Pool</t>
+  </si>
+  <si>
+    <t>Heavy Magic Skill Pool</t>
+  </si>
+  <si>
+    <t>Holy Greave</t>
+  </si>
+  <si>
+    <t>Cosmos Lighting</t>
+  </si>
+  <si>
+    <t>Nature's Command</t>
+  </si>
+  <si>
+    <t>Summon Souroff</t>
+  </si>
+  <si>
+    <t>Summon a Souroff near the enemies</t>
+  </si>
+  <si>
+    <t>Healing the team and remove stun</t>
+  </si>
+  <si>
+    <t>Stun all other characters</t>
+  </si>
+  <si>
+    <t>Be invisible while turning all the tiles into falling rock</t>
+  </si>
+  <si>
+    <t>Rage</t>
+  </si>
+  <si>
+    <t>Guardian</t>
+  </si>
+  <si>
+    <t>Speed up self 2 point</t>
+  </si>
+  <si>
+    <t>Heal up self 3 point</t>
+  </si>
+  <si>
+    <t>Damage and Power up self 1 point</t>
+  </si>
+  <si>
+    <t>Guard up self 3 point</t>
+  </si>
+  <si>
+    <t>Boost</t>
   </si>
 </sst>
 </file>
@@ -507,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +798,7 @@
         <v>6</v>
       </c>
       <c r="F13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G13">
         <v>5.5</v>
@@ -925,12 +976,215 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" t="s">
+        <v>50</v>
+      </c>
+      <c r="N6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>